<commit_message>
changed AD_GWAS_diff_rhythms xlsx files
</commit_message>
<xml_diff>
--- a/Cyclops_ordering/downstream_output_Mglia_all/AD_GWAS_diff_rhythms_CyclingBHQ1.xlsx
+++ b/Cyclops_ordering/downstream_output_Mglia_all/AD_GWAS_diff_rhythms_CyclingBHQ1.xlsx
@@ -11,6 +11,7 @@
     <sheet name="GWAS_AD_cycling" sheetId="2" r:id="rId2"/>
     <sheet name="GWAS_diff_rhyth" sheetId="3" r:id="rId3"/>
     <sheet name="GWAS_diff_mesor" sheetId="4" r:id="rId4"/>
+    <sheet name="GWAS_diff_expr" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -354,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -968,29 +969,29 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>APH1B</t>
+          <t>PSEN1</t>
         </is>
       </c>
       <c r="B20">
-        <v>4.37213686937034</v>
+        <v>6.05233824970298</v>
       </c>
       <c r="C20">
-        <v>3.98711834917171</v>
+        <v>8.64101421063647</v>
       </c>
       <c r="D20">
-        <v>0.0202804605758647</v>
+        <v>0.00171277736622371</v>
       </c>
       <c r="E20">
-        <v>0.0893860195149267</v>
+        <v>0.0688167975031598</v>
       </c>
       <c r="F20">
-        <v>-3.75853908620031</v>
+        <v>-1.97708300155701</v>
       </c>
       <c r="G20">
-        <v>-1.33060011566445</v>
+        <v>8.41179347068007</v>
       </c>
       <c r="H20">
-        <v>0.0548566068989192</v>
+        <v>0.008430288903006721</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -999,29 +1000,29 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CTSH</t>
+          <t>APH1B</t>
         </is>
       </c>
       <c r="B21">
-        <v>2.16645652080834</v>
+        <v>4.37213686937034</v>
       </c>
       <c r="C21">
-        <v>5.9329684754379</v>
+        <v>3.98711834917171</v>
       </c>
       <c r="D21">
-        <v>0.0288756775211734</v>
+        <v>0.0202804605758647</v>
       </c>
       <c r="E21">
-        <v>0.07097772865229959</v>
+        <v>0.0893860195149267</v>
       </c>
       <c r="F21">
-        <v>4.91118240349625</v>
+        <v>-3.75853908620031</v>
       </c>
       <c r="G21">
-        <v>-3.32872382905653</v>
+        <v>-1.33060011566445</v>
       </c>
       <c r="H21">
-        <v>0.07274903613946911</v>
+        <v>0.0548566068989192</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -1030,29 +1031,29 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>DOC2A</t>
+          <t>CTSH</t>
         </is>
       </c>
       <c r="B22">
-        <v>1.73933888784861</v>
+        <v>2.16645652080834</v>
       </c>
       <c r="C22">
-        <v>5.28182425179453</v>
+        <v>5.9329684754379</v>
       </c>
       <c r="D22">
-        <v>0.0211408758493537</v>
+        <v>0.0288756775211734</v>
       </c>
       <c r="E22">
-        <v>0.106308860713673</v>
+        <v>0.07097772865229959</v>
       </c>
       <c r="F22">
-        <v>5.20698234978855</v>
+        <v>4.91118240349625</v>
       </c>
       <c r="G22">
-        <v>-0.886003519087449</v>
+        <v>-3.32872382905653</v>
       </c>
       <c r="H22">
-        <v>0.0566385708940188</v>
+        <v>0.07274903613946911</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -1061,29 +1062,29 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>MAF</t>
+          <t>DOC2A</t>
         </is>
       </c>
       <c r="B23">
-        <v>4.06789600894764</v>
+        <v>1.73933888784861</v>
       </c>
       <c r="C23">
-        <v>51.7182462143413</v>
+        <v>5.28182425179453</v>
       </c>
       <c r="D23">
-        <v>0.00264744399497033</v>
+        <v>0.0211408758493537</v>
       </c>
       <c r="E23">
-        <v>0.114443501062927</v>
+        <v>0.106308860713673</v>
       </c>
       <c r="F23">
-        <v>-41.3437981866802</v>
+        <v>5.20698234978855</v>
       </c>
       <c r="G23">
-        <v>-31.0719703750228</v>
+        <v>-0.886003519087449</v>
       </c>
       <c r="H23">
-        <v>0.0116901237151926</v>
+        <v>0.0566385708940188</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -1092,29 +1093,29 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>PLCG2</t>
+          <t>MAF</t>
         </is>
       </c>
       <c r="B24">
-        <v>5.18054180169089</v>
+        <v>4.06789600894764</v>
       </c>
       <c r="C24">
-        <v>20.1038849580489</v>
+        <v>51.7182462143413</v>
       </c>
       <c r="D24">
-        <v>0.00094097817324376</v>
+        <v>0.00264744399497033</v>
       </c>
       <c r="E24">
-        <v>0.0681993192523138</v>
+        <v>0.114443501062927</v>
       </c>
       <c r="F24">
-        <v>-17.9407738537668</v>
+        <v>-41.3437981866802</v>
       </c>
       <c r="G24">
-        <v>9.071649460514911</v>
+        <v>-31.0719703750228</v>
       </c>
       <c r="H24">
-        <v>0.00540418503188178</v>
+        <v>0.0116901237151926</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -1123,29 +1124,29 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>WDR81</t>
+          <t>PLCG2</t>
         </is>
       </c>
       <c r="B25">
-        <v>6.04339577655414</v>
+        <v>5.18054180169089</v>
       </c>
       <c r="C25">
-        <v>3.90817426035415</v>
+        <v>20.1038849580489</v>
       </c>
       <c r="D25">
-        <v>0.00122946069159365</v>
+        <v>0.00094097817324376</v>
       </c>
       <c r="E25">
-        <v>0.118409040173526</v>
+        <v>0.0681993192523138</v>
       </c>
       <c r="F25">
-        <v>-0.928184290636255</v>
+        <v>-17.9407738537668</v>
       </c>
       <c r="G25">
-        <v>3.79635350987112</v>
+        <v>9.071649460514911</v>
       </c>
       <c r="H25">
-        <v>0.00660066276864022</v>
+        <v>0.00540418503188178</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -1154,29 +1155,29 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SCIMP</t>
+          <t>WDR81</t>
         </is>
       </c>
       <c r="B26">
-        <v>5.14484149849709</v>
+        <v>6.04339577655414</v>
       </c>
       <c r="C26">
-        <v>3.80027306754704</v>
+        <v>3.90817426035415</v>
       </c>
       <c r="D26">
-        <v>0.00815911710524185</v>
+        <v>0.00122946069159365</v>
       </c>
       <c r="E26">
-        <v>0.128039091271394</v>
+        <v>0.118409040173526</v>
       </c>
       <c r="F26">
-        <v>-3.45042233780339</v>
+        <v>-0.928184290636255</v>
       </c>
       <c r="G26">
-        <v>1.59268988780327</v>
+        <v>3.79635350987112</v>
       </c>
       <c r="H26">
-        <v>0.0273911168619209</v>
+        <v>0.00660066276864022</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -1185,29 +1186,29 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GRN</t>
+          <t>SCIMP</t>
         </is>
       </c>
       <c r="B27">
-        <v>2.97668356277389</v>
+        <v>5.14484149849709</v>
       </c>
       <c r="C27">
-        <v>11.7074612300916</v>
+        <v>3.80027306754704</v>
       </c>
       <c r="D27">
-        <v>0.0002027387530325</v>
+        <v>0.00815911710524185</v>
       </c>
       <c r="E27">
-        <v>0.126064798078113</v>
+        <v>0.128039091271394</v>
       </c>
       <c r="F27">
-        <v>1.92192792848848</v>
+        <v>-3.45042233780339</v>
       </c>
       <c r="G27">
-        <v>-11.5486294204895</v>
+        <v>1.59268988780327</v>
       </c>
       <c r="H27">
-        <v>0.00164237305361615</v>
+        <v>0.0273911168619209</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -1216,29 +1217,29 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ABCA7</t>
+          <t>GRN</t>
         </is>
       </c>
       <c r="B28">
-        <v>0.672656758430218</v>
+        <v>2.97668356277389</v>
       </c>
       <c r="C28">
-        <v>3.37578688336286</v>
+        <v>11.7074612300916</v>
       </c>
       <c r="D28">
-        <v>0.00049361871352716</v>
+        <v>0.0002027387530325</v>
       </c>
       <c r="E28">
-        <v>0.220608155401612</v>
+        <v>0.126064798078113</v>
       </c>
       <c r="F28">
-        <v>2.10333876562959</v>
+        <v>1.92192792848848</v>
       </c>
       <c r="G28">
-        <v>2.64043616072885</v>
+        <v>-11.5486294204895</v>
       </c>
       <c r="H28">
-        <v>0.00322032263176092</v>
+        <v>0.00164237305361615</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -1247,29 +1248,29 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>KLF16</t>
+          <t>ABCA7</t>
         </is>
       </c>
       <c r="B29">
-        <v>2.31169882912982</v>
+        <v>0.672656758430218</v>
       </c>
       <c r="C29">
-        <v>2.17588592373327</v>
+        <v>3.37578688336286</v>
       </c>
       <c r="D29">
-        <v>0.0444504054025835</v>
+        <v>0.00049361871352716</v>
       </c>
       <c r="E29">
-        <v>0.100378682826478</v>
+        <v>0.220608155401612</v>
       </c>
       <c r="F29">
-        <v>1.60549856027429</v>
+        <v>2.10333876562959</v>
       </c>
       <c r="G29">
-        <v>-1.46862313956227</v>
+        <v>2.64043616072885</v>
       </c>
       <c r="H29">
-        <v>0.0999722577538107</v>
+        <v>0.00322032263176092</v>
       </c>
       <c r="I29">
         <v>1</v>
@@ -1278,31 +1279,93 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>KLF16</t>
+        </is>
+      </c>
+      <c r="B30">
+        <v>2.31169882912982</v>
+      </c>
+      <c r="C30">
+        <v>2.17588592373327</v>
+      </c>
+      <c r="D30">
+        <v>0.0444504054025835</v>
+      </c>
+      <c r="E30">
+        <v>0.100378682826478</v>
+      </c>
+      <c r="F30">
+        <v>1.60549856027429</v>
+      </c>
+      <c r="G30">
+        <v>-1.46862313956227</v>
+      </c>
+      <c r="H30">
+        <v>0.0999722577538107</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>APOE</t>
+        </is>
+      </c>
+      <c r="B31">
+        <v>2.02302671405073</v>
+      </c>
+      <c r="C31">
+        <v>86.2726781633761</v>
+      </c>
+      <c r="D31">
+        <v>3.88998002072418E-07</v>
+      </c>
+      <c r="E31">
+        <v>0.260421021960011</v>
+      </c>
+      <c r="F31">
+        <v>77.6000931968085</v>
+      </c>
+      <c r="G31">
+        <v>-37.6988134206916</v>
+      </c>
+      <c r="H31">
+        <v>1.56105878898893E-05</v>
+      </c>
+      <c r="I31">
+        <v>0.00371531991779366</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>APP</t>
         </is>
       </c>
-      <c r="B30">
+      <c r="B32">
         <v>2.29569813409687</v>
       </c>
-      <c r="C30">
+      <c r="C32">
         <v>14.7149259686369</v>
       </c>
-      <c r="D30">
+      <c r="D32">
         <v>0.0184456658506072</v>
       </c>
-      <c r="E30">
+      <c r="E32">
         <v>0.06813294559862371</v>
       </c>
-      <c r="F30">
+      <c r="F32">
         <v>11.015071691962</v>
       </c>
-      <c r="G30">
+      <c r="G32">
         <v>-9.75690739340097</v>
       </c>
-      <c r="H30">
+      <c r="H32">
         <v>0.0510502910863951</v>
       </c>
-      <c r="I30">
+      <c r="I32">
         <v>1</v>
       </c>
     </row>
@@ -1313,7 +1376,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2079,6 +2142,37 @@
         <v>1</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>APOE</t>
+        </is>
+      </c>
+      <c r="B25">
+        <v>1.88985524851238</v>
+      </c>
+      <c r="C25">
+        <v>127.653930417555</v>
+      </c>
+      <c r="D25">
+        <v>7.28876513091738E-07</v>
+      </c>
+      <c r="E25">
+        <v>0.357872140519487</v>
+      </c>
+      <c r="F25">
+        <v>121.211367964314</v>
+      </c>
+      <c r="G25">
+        <v>-40.0416062024206</v>
+      </c>
+      <c r="H25">
+        <v>4.76815039488986E-05</v>
+      </c>
+      <c r="I25">
+        <v>0.00696149957653919</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2086,7 +2180,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2125,1383 +2219,153 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Log_AD_CTL_ampRatio</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>BHQ</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Bonf</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Log_AD_CTL_ampRatio</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SORT1</t>
+          <t>RASGEF1C</t>
         </is>
       </c>
       <c r="B2">
-        <v>0.732371062478049</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1.39391656795109</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1.00331022796921</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>21.5590854321101</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>17.0304224452205</t>
-        </is>
+        <v>0.69870507776736</v>
+      </c>
+      <c r="C2">
+        <v>4.4805897590458</v>
+      </c>
+      <c r="D2">
+        <v>4.63770427565182</v>
+      </c>
+      <c r="E2">
+        <v>85.579745735117</v>
+      </c>
+      <c r="F2">
+        <v>65.2596216749329</v>
       </c>
       <c r="G2">
-        <v>0.9037289811140788</v>
+        <v>0.271075145954422</v>
       </c>
       <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0.2357960251695227</v>
+        <v>0.8733813472092</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PRKD3</t>
+          <t>SPDYE3</t>
         </is>
       </c>
       <c r="B3">
-        <v>0.649276683392797</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1.34875227856164</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1.18047884899807</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>30.8912289653309</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>20.4985181842062</t>
-        </is>
+        <v>0.907396955477238</v>
+      </c>
+      <c r="C3">
+        <v>4.93521282057408</v>
+      </c>
+      <c r="D3">
+        <v>5.02315082895087</v>
+      </c>
+      <c r="E3">
+        <v>6.31906393677738</v>
+      </c>
+      <c r="F3">
+        <v>5.97048907206786</v>
       </c>
       <c r="G3">
-        <v>0.9037289811140788</v>
+        <v>0.0567422402512817</v>
       </c>
       <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0.4101196915208483</v>
+        <v>0.907396955477238</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NCK2</t>
+          <t>MS4A4A</t>
         </is>
       </c>
       <c r="B4">
-        <v>0.366116525066049</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.900198035964252</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1.5507337087456</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>89.2053394723794</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>58.6113117315709</t>
-        </is>
+        <v>0.502534748578515</v>
+      </c>
+      <c r="C4">
+        <v>1.17228693959922</v>
+      </c>
+      <c r="D4">
+        <v>1.13122163417065</v>
+      </c>
+      <c r="E4">
+        <v>21.6688042113024</v>
+      </c>
+      <c r="F4">
+        <v>13.123784969381</v>
       </c>
       <c r="G4">
-        <v>0.8681621914167958</v>
+        <v>0.501447401836594</v>
       </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>0.4200131864338122</v>
+        <v>0.837557914297525</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>WDR12</t>
+          <t>ABCA7</t>
         </is>
       </c>
       <c r="B5">
-        <v>0.0382241486422535</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>5.09058646443008</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>4.51397473428338</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>7.69093642851817</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2.32391583061898</t>
-        </is>
+        <v>0.0543963626276233</v>
+      </c>
+      <c r="C5">
+        <v>1.62873904263362</v>
+      </c>
+      <c r="D5">
+        <v>0.672796080442663</v>
+      </c>
+      <c r="E5">
+        <v>4.07987242509666</v>
+      </c>
+      <c r="F5">
+        <v>3.41025637450735</v>
       </c>
       <c r="G5">
-        <v>0.3902948969567246</v>
+        <v>0.179278247959243</v>
       </c>
       <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1.196788927470865</v>
+        <v>0.2719818131381165</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>INPP5D</t>
+          <t>APOE</t>
         </is>
       </c>
       <c r="B6">
-        <v>0.47231390524542</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>5.02024770561303</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>5.31723742347952</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>27.7337389895786</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>57.6365807626063</t>
-        </is>
+        <v>0.186175053768831</v>
+      </c>
+      <c r="C6">
+        <v>1.89701676415387</v>
+      </c>
+      <c r="D6">
+        <v>2.01490266472496</v>
+      </c>
+      <c r="E6">
+        <v>130.306309513959</v>
+      </c>
+      <c r="F6">
+        <v>84.4682749423154</v>
       </c>
       <c r="G6">
-        <v>0.8700519307152473</v>
+        <v>0.433511886539307</v>
       </c>
       <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>-0.731507762726163</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>RHOH</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>0.211424969162916</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0.743213453258984</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>5.85122451156744</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>7.03584469225168</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>3.11017252279913</t>
-        </is>
-      </c>
-      <c r="G7">
-        <v>0.82220821341134</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>0.8163395551089465</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ANKH</t>
-        </is>
-      </c>
-      <c r="B8">
-        <v>0.421678778688158</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>4.80701098770533</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>4.64573789902144</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>18.1713780172057</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>10.2888733826833</t>
-        </is>
-      </c>
-      <c r="G8">
-        <v>0.8681621914167958</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>0.5687846625426631</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>COX7C</t>
-        </is>
-      </c>
-      <c r="B9">
-        <v>0.149434634579102</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>3.53817419912885</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2.99339443711743</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>9.1044517157029</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>21.7103528088164</t>
-        </is>
-      </c>
-      <c r="G9">
-        <v>0.7432003263737674</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>-0.869025741308508</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>TNIP1</t>
-        </is>
-      </c>
-      <c r="B10">
-        <v>0.421667655699681</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2.11406367820784</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1.32159339170617</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2.83744552285584</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2.37371279243214</t>
-        </is>
-      </c>
-      <c r="G10">
-        <v>0.8681621914167958</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>0.1784488752023191</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>RASGEF1C</t>
-        </is>
-      </c>
-      <c r="B11">
-        <v>0.69870507776736</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>4.4805897590458</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>4.63770427565182</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>85.579745735117</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>65.2596216749329</t>
-        </is>
-      </c>
-      <c r="G11">
-        <v>0.9037289811140788</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>0.2710751459544223</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>TREM2</t>
-        </is>
-      </c>
-      <c r="B12">
-        <v>0.28180916297776</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>3.64525368939168</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>3.00736900951015</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>7.85969653191116</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>10.9171113771563</t>
-        </is>
-      </c>
-      <c r="G12">
-        <v>0.8681621914167958</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>-0.3285834128980198</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>UMAD1</t>
-        </is>
-      </c>
-      <c r="B13">
-        <v>0.748804012923094</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1.40794760217862</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>1.39130506617061</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>20.5749120059922</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>14.490106297959</t>
-        </is>
-      </c>
-      <c r="G13">
-        <v>0.9037289811140788</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>0.350606377551303</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>ICA1</t>
-        </is>
-      </c>
-      <c r="B14">
-        <v>0.906777975000568</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>4.61646697011687</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>4.48016579918455</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>8.10149713345091</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>6.52931488752623</t>
-        </is>
-      </c>
-      <c r="G14">
-        <v>0.910262187902068</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>0.2157468557889147</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>SEC61G</t>
-        </is>
-      </c>
-      <c r="B15">
-        <v>0.901198755768749</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>2.85600973128439</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>2.9112702698288</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>3.16767018659603</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>3.95898821785669</t>
-        </is>
-      </c>
-      <c r="G15">
-        <v>0.910262187902068</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>-0.2229921313131401</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>SPDYE3</t>
-        </is>
-      </c>
-      <c r="B16">
-        <v>0.907396955477238</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>4.93521282057408</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>5.02315082895087</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>6.31906393677738</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>5.97048907206786</t>
-        </is>
-      </c>
-      <c r="G16">
-        <v>0.910262187902068</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>0.05674224025128172</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>CTSB</t>
-        </is>
-      </c>
-      <c r="B17">
-        <v>0.386932767291086</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>1.81371433666015</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>1.97855695551837</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>75.7192646580687</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>39.6325537281704</t>
-        </is>
-      </c>
-      <c r="G17">
-        <v>0.8681621914167958</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>0.6473817705699464</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>CLU</t>
-        </is>
-      </c>
-      <c r="B18">
-        <v>0.0448889463060818</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>3.77756319934017</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2.24577315699528</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>33.3753077820444</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>35.3992463259049</t>
-        </is>
-      </c>
-      <c r="G18">
-        <v>0.3902948969567246</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>-0.05887419107260696</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>ANK3</t>
-        </is>
-      </c>
-      <c r="B19">
-        <v>0.27377966880573</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>4.80163804717701</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>5.51544056521126</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>13.1138579872485</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>12.6964427683294</t>
-        </is>
-      </c>
-      <c r="G19">
-        <v>0.8681621914167958</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>0.03234767543969521</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>TSPAN14</t>
-        </is>
-      </c>
-      <c r="B20">
-        <v>0.471055367402235</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>0.629593555463485</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>0.121784097545303</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>20.9645256751127</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>19.7766949935117</t>
-        </is>
-      </c>
-      <c r="G20">
-        <v>0.8700519307152473</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>0.05832753182161766</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>BLNK</t>
-        </is>
-      </c>
-      <c r="B21">
-        <v>0.910262187902068</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>4.60818974449759</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>4.49401118378777</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>43.4299388916471</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>51.0752315993771</t>
-        </is>
-      </c>
-      <c r="G21">
-        <v>0.910262187902068</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>-0.1621506356974915</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>MS4A4A</t>
-        </is>
-      </c>
-      <c r="B22">
-        <v>0.502534748578515</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>1.17228693959922</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>1.13122163417065</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>21.6688042113024</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>13.123784969381</t>
-        </is>
-      </c>
-      <c r="G22">
-        <v>0.8794358100124012</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <v>0.5014474018365935</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>SORL1</t>
-        </is>
-      </c>
-      <c r="B23">
-        <v>0.419220957611374</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>4.1094679758933</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>4.64854039553335</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>156.052723221402</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>133.204225029976</t>
-        </is>
-      </c>
-      <c r="G23">
-        <v>0.8681621914167958</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>0.1583104424712144</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>TPCN1</t>
-        </is>
-      </c>
-      <c r="B24">
-        <v>0.655391008800433</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>4.5458477549679</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>4.76056550782716</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>15.1405076503535</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>11.4787649558618</t>
-        </is>
-      </c>
-      <c r="G24">
-        <v>0.9037289811140788</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24">
-        <v>0.2768749749915787</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>MINDY2</t>
-        </is>
-      </c>
-      <c r="B25">
-        <v>0.0586255310580753</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>4.61165409560028</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>5.86957404820501</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>8.89256083847719</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>3.67422361771227</t>
-        </is>
-      </c>
-      <c r="G25">
-        <v>0.3902948969567246</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>0.8838732165066715</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>APH1B</t>
-        </is>
-      </c>
-      <c r="B26">
-        <v>0.896738866288593</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>4.17749768089018</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>4.43461524977715</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>3.43476285363536</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>4.00251927029169</t>
-        </is>
-      </c>
-      <c r="G26">
-        <v>0.910262187902068</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="I26">
-        <v>-0.1529760953928805</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>CTSH</t>
-        </is>
-      </c>
-      <c r="B27">
-        <v>0.0624958498489298</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>1.07768961985323</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2.19175101722477</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>8.13106789348246</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>5.92395950063119</t>
-        </is>
-      </c>
-      <c r="G27">
-        <v>0.3902948969567246</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <v>0.3166872072538001</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>DOC2A</t>
-        </is>
-      </c>
-      <c r="B28">
-        <v>0.363006927587269</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>2.44578991684332</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>1.73366770187174</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>5.65508663251558</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>5.40908444096408</t>
-        </is>
-      </c>
-      <c r="G28">
-        <v>0.8681621914167958</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-      <c r="I28">
-        <v>0.04447558511779647</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>MAF</t>
-        </is>
-      </c>
-      <c r="B29">
-        <v>0.6639338856720099</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>4.05981853699267</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>4.04612694986241</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>72.1042990704968</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>52.2305244007489</t>
-        </is>
-      </c>
-      <c r="G29">
-        <v>0.9037289811140788</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <v>0.3224465863922686</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>PLCG2</t>
-        </is>
-      </c>
-      <c r="B30">
-        <v>0.661530742474091</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>5.10696467693298</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>5.12581182655027</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>10.720459248323</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>19.0926958423024</t>
-        </is>
-      </c>
-      <c r="G30">
-        <v>0.9037289811140788</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-      <c r="I30">
-        <v>-0.5771518502256409</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>WDR81</t>
-        </is>
-      </c>
-      <c r="B31">
-        <v>0.728408553579916</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>5.93529480554246</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>6.05339161554498</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>2.48109751026355</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>3.79908655667701</t>
-        </is>
-      </c>
-      <c r="G31">
-        <v>0.9037289811140788</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="I31">
-        <v>-0.4260596512705602</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>SCIMP</t>
-        </is>
-      </c>
-      <c r="B32">
-        <v>0.788312284876445</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>4.95683101536233</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>5.10317004652706</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>4.77051219937732</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>3.56760767136573</t>
-        </is>
-      </c>
-      <c r="G32">
-        <v>0.910262187902068</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="I32">
-        <v>0.2905584273647726</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>GRN</t>
-        </is>
-      </c>
-      <c r="B33">
-        <v>0.169874360314004</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>2.68475725672341</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>2.99083821965921</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>19.7917378970758</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>11.4497836350901</t>
-        </is>
-      </c>
-      <c r="G33">
-        <v>0.7432003263737674</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <v>0.5472937393673386</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>ABCA7</t>
-        </is>
-      </c>
-      <c r="B34">
-        <v>0.0543963626276233</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>1.62873904263362</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>0.672796080442663</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>4.07987242509666</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>3.41025637450735</t>
-        </is>
-      </c>
-      <c r="G34">
-        <v>0.3902948969567246</v>
-      </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-      <c r="I34">
-        <v>0.1792782479592431</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>KLF16</t>
-        </is>
-      </c>
-      <c r="B35">
-        <v>0.586219608490758</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>1.97479988384536</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>2.289678952817</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>3.27496179257352</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>2.20781577485639</t>
-        </is>
-      </c>
-      <c r="G35">
-        <v>0.9037289811140788</v>
-      </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="I35">
-        <v>0.394302512996015</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>APP</t>
-        </is>
-      </c>
-      <c r="B36">
-        <v>0.0669076966211528</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>3.56173724740052</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>2.26223223650322</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>16.4344005938127</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>14.5945634616444</t>
-        </is>
-      </c>
-      <c r="G36">
-        <v>0.3902948969567246</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36">
-        <v>0.1187276414002695</v>
+        <v>0.4654376344220775</v>
       </c>
     </row>
   </sheetData>
@@ -3511,7 +2375,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3543,11 +2407,6 @@
           <t>BHQ</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Bonf</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3565,10 +2424,7 @@
         <v>268.059905069876</v>
       </c>
       <c r="E2">
-        <v>0.7898664528985569</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
+        <v>0.7494294275918612</v>
       </c>
     </row>
     <row r="3">
@@ -3587,10 +2443,7 @@
         <v>158.357170206531</v>
       </c>
       <c r="E3">
-        <v>0.95738442394733</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="4">
@@ -3609,10 +2462,7 @@
         <v>196.125260631337</v>
       </c>
       <c r="E4">
-        <v>0.977580139164912</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="5">
@@ -3631,10 +2481,7 @@
         <v>601.71975063326</v>
       </c>
       <c r="E5">
-        <v>0.9881032566671329</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="6">
@@ -3653,10 +2500,7 @@
         <v>315.259700112467</v>
       </c>
       <c r="E6">
-        <v>0.636562823120952</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
+        <v>0.6963558963132086</v>
       </c>
     </row>
     <row r="7">
@@ -3675,10 +2519,7 @@
         <v>42.1770075105111</v>
       </c>
       <c r="E7">
-        <v>0.975583930969828</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="8">
@@ -3697,10 +2538,7 @@
         <v>746.23151759667</v>
       </c>
       <c r="E8">
-        <v>0.845212988555911</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
+        <v>0.7529122425565569</v>
       </c>
     </row>
     <row r="9">
@@ -3719,10 +2557,7 @@
         <v>16.6032010157338</v>
       </c>
       <c r="E9">
-        <v>0.848684779549214</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
+        <v>0.7529122425565569</v>
       </c>
     </row>
     <row r="10">
@@ -3741,10 +2576,7 @@
         <v>56.489501021142</v>
       </c>
       <c r="E10">
-        <v>0.897442001001996</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
+        <v>0.7765096633414705</v>
       </c>
     </row>
     <row r="11">
@@ -3763,10 +2595,7 @@
         <v>157.620457730767</v>
       </c>
       <c r="E11">
-        <v>0.723680870383996</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
+        <v>0.742295706874482</v>
       </c>
     </row>
     <row r="12">
@@ -3785,10 +2614,7 @@
         <v>157.696602180942</v>
       </c>
       <c r="E12">
-        <v>0.7947476887048101</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
+        <v>0.7494294275918612</v>
       </c>
     </row>
     <row r="13">
@@ -3807,10 +2633,7 @@
         <v>32.4326989313832</v>
       </c>
       <c r="E13">
-        <v>0.901746868915468</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
+        <v>0.7765096633414705</v>
       </c>
     </row>
     <row r="14">
@@ -3829,10 +2652,7 @@
         <v>334.792855757414</v>
       </c>
       <c r="E14">
-        <v>0.424562488937702</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
+        <v>0.6963558963132086</v>
       </c>
     </row>
     <row r="15">
@@ -3851,10 +2671,7 @@
         <v>32.916484488737</v>
       </c>
       <c r="E15">
-        <v>0.896373494661575</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
+        <v>0.7765096633414705</v>
       </c>
     </row>
     <row r="16">
@@ -3873,10 +2690,7 @@
         <v>61.4342704475984</v>
       </c>
       <c r="E16">
-        <v>0.991549575772422</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
+        <v>0.9225493509511271</v>
       </c>
     </row>
     <row r="17">
@@ -3895,10 +2709,7 @@
         <v>152.935079398903</v>
       </c>
       <c r="E17">
-        <v>0.884079306261918</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
+        <v>0.7765096633414705</v>
       </c>
     </row>
     <row r="18">
@@ -3917,10 +2728,7 @@
         <v>235.327661183782</v>
       </c>
       <c r="E18">
-        <v>0.989255647653869</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="19">
@@ -3939,10 +2747,7 @@
         <v>69.9981533152599</v>
       </c>
       <c r="E19">
-        <v>0.955803777381604</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="20">
@@ -3961,10 +2766,7 @@
         <v>61.3804126684608</v>
       </c>
       <c r="E20">
-        <v>0.993594698777889</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
+        <v>0.93706784747669</v>
       </c>
     </row>
     <row r="21">
@@ -3983,10 +2785,7 @@
         <v>1021.50290499017</v>
       </c>
       <c r="E21">
-        <v>0.730603035166028</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
+        <v>0.742295706874482</v>
       </c>
     </row>
     <row r="22">
@@ -4005,10 +2804,7 @@
         <v>33.6357736008635</v>
       </c>
       <c r="E22">
-        <v>0.987168343489203</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="23">
@@ -4027,10 +2823,7 @@
         <v>30.9145870584843</v>
       </c>
       <c r="E23">
-        <v>0.920268708275661</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
+        <v>0.7765096633414705</v>
       </c>
     </row>
     <row r="24">
@@ -4049,10 +2842,7 @@
         <v>18.1970915648495</v>
       </c>
       <c r="E24">
-        <v>0.9221030802360149</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
+        <v>0.7854973895780016</v>
       </c>
     </row>
     <row r="25">
@@ -4071,10 +2861,7 @@
         <v>508.30222475707</v>
       </c>
       <c r="E25">
-        <v>0.920268708275661</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
+        <v>0.7765096633414705</v>
       </c>
     </row>
     <row r="26">
@@ -4093,10 +2880,7 @@
         <v>188.898223441643</v>
       </c>
       <c r="E26">
-        <v>0.942557800919317</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
+        <v>0.860561924921978</v>
       </c>
     </row>
     <row r="27">
@@ -4115,10 +2899,7 @@
         <v>481.251290942092</v>
       </c>
       <c r="E27">
-        <v>0.9874549941408099</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="28">
@@ -4137,10 +2918,7 @@
         <v>24.4809275225977</v>
       </c>
       <c r="E28">
-        <v>0.973881012141923</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="29">
@@ -4159,10 +2937,7 @@
         <v>117.453691273994</v>
       </c>
       <c r="E29">
-        <v>0.909590710562131</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
+        <v>0.7765096633414705</v>
       </c>
     </row>
     <row r="30">
@@ -4181,10 +2956,7 @@
         <v>335.74563685961</v>
       </c>
       <c r="E30">
-        <v>0.834344952739362</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
+        <v>0.7529122425565569</v>
       </c>
     </row>
     <row r="31">
@@ -4203,10 +2975,7 @@
         <v>132.348440323693</v>
       </c>
       <c r="E31">
-        <v>0.9191799049368</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
+        <v>0.7765096633414705</v>
       </c>
     </row>
     <row r="32">
@@ -4225,10 +2994,7 @@
         <v>216.370388297515</v>
       </c>
       <c r="E32">
-        <v>0.663712448300777</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
+        <v>0.6963558963132086</v>
       </c>
     </row>
     <row r="33">
@@ -4247,10 +3013,7 @@
         <v>428.982871556424</v>
       </c>
       <c r="E33">
-        <v>0.788771042745505</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
+        <v>0.7494294275918612</v>
       </c>
     </row>
     <row r="34">
@@ -4269,10 +3032,7 @@
         <v>104.416915799944</v>
       </c>
       <c r="E34">
-        <v>0.746718322854502</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
+        <v>0.7494294275918612</v>
       </c>
     </row>
     <row r="35">
@@ -4291,10 +3051,7 @@
         <v>83.2112376840777</v>
       </c>
       <c r="E35">
-        <v>0.96381647125748</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="36">
@@ -4313,10 +3070,7 @@
         <v>83.3658611958806</v>
       </c>
       <c r="E36">
-        <v>0.891559626726243</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
+        <v>0.7765096633414705</v>
       </c>
     </row>
     <row r="37">
@@ -4335,10 +3089,7 @@
         <v>79.009631401823</v>
       </c>
       <c r="E37">
-        <v>0.808827048458178</v>
-      </c>
-      <c r="F37">
-        <v>1</v>
+        <v>0.7529122425565569</v>
       </c>
     </row>
     <row r="38">
@@ -4357,10 +3108,7 @@
         <v>1425.21509710123</v>
       </c>
       <c r="E38">
-        <v>0.943188682530141</v>
-      </c>
-      <c r="F38">
-        <v>1</v>
+        <v>0.8629860577832271</v>
       </c>
     </row>
     <row r="39">
@@ -4379,10 +3127,7 @@
         <v>103.874316696888</v>
       </c>
       <c r="E39">
-        <v>0.895627722867024</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
+        <v>0.7765096633414705</v>
       </c>
     </row>
     <row r="40">
@@ -4401,428 +3146,1771 @@
         <v>21.8590703513042</v>
       </c>
       <c r="E40">
-        <v>0.664901170173695</v>
-      </c>
-      <c r="F40">
-        <v>1</v>
+        <v>0.6963558963132086</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>SPPL2A</t>
+          <t>PSEN1</t>
         </is>
       </c>
       <c r="B41">
-        <v>0.326261971774508</v>
+        <v>0.325992558237467</v>
       </c>
       <c r="C41">
-        <v>95.2607933692821</v>
+        <v>125.7243355273</v>
       </c>
       <c r="D41">
-        <v>96.5168881051724</v>
+        <v>127.413129695006</v>
       </c>
       <c r="E41">
-        <v>0.867395346092419</v>
-      </c>
-      <c r="F41">
-        <v>1</v>
+        <v>0.7529122425565569</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>MINDY2</t>
+          <t>SPPL2A</t>
         </is>
       </c>
       <c r="B42">
-        <v>0.08124152123654101</v>
+        <v>0.326261971774508</v>
       </c>
       <c r="C42">
-        <v>98.076810566912</v>
+        <v>95.2607933692821</v>
       </c>
       <c r="D42">
-        <v>101.111508351686</v>
+        <v>96.5168881051724</v>
       </c>
       <c r="E42">
-        <v>0.667300434212906</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
+        <v>0.7529122425565569</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>APH1B</t>
+          <t>MINDY2</t>
         </is>
       </c>
       <c r="B43">
-        <v>0.118331978423143</v>
+        <v>0.08124152123654101</v>
       </c>
       <c r="C43">
-        <v>44.55383656947</v>
+        <v>98.076810566912</v>
       </c>
       <c r="D43">
-        <v>46.256590531449</v>
+        <v>101.111508351686</v>
       </c>
       <c r="E43">
-        <v>0.725953935618223</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
+        <v>0.6963558963132086</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>SNX1</t>
+          <t>APH1B</t>
         </is>
       </c>
       <c r="B44">
-        <v>0.805612394899478</v>
+        <v>0.118331978423143</v>
       </c>
       <c r="C44">
-        <v>133.569492523061</v>
+        <v>44.55383656947</v>
       </c>
       <c r="D44">
-        <v>131.833313091111</v>
+        <v>46.256590531449</v>
       </c>
       <c r="E44">
-        <v>0.975241839826345</v>
-      </c>
-      <c r="F44">
-        <v>1</v>
+        <v>0.742295706874482</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CTSH</t>
+          <t>SNX1</t>
         </is>
       </c>
       <c r="B45">
-        <v>0.79077607052319</v>
+        <v>0.805612394899478</v>
       </c>
       <c r="C45">
-        <v>82.9592615094008</v>
+        <v>133.569492523061</v>
       </c>
       <c r="D45">
-        <v>82.1731366217701</v>
+        <v>131.833313091111</v>
       </c>
       <c r="E45">
-        <v>0.973881012141923</v>
-      </c>
-      <c r="F45">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>DOC2A</t>
+          <t>CTSH</t>
         </is>
       </c>
       <c r="B46">
-        <v>0.321582034841199</v>
+        <v>0.79077607052319</v>
       </c>
       <c r="C46">
-        <v>50.0226708720351</v>
+        <v>82.9592615094008</v>
       </c>
       <c r="D46">
-        <v>54.4925966516079</v>
+        <v>82.1731366217701</v>
       </c>
       <c r="E46">
-        <v>0.86351527343641</v>
-      </c>
-      <c r="F46">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>MAF</t>
+          <t>DOC2A</t>
         </is>
       </c>
       <c r="B47">
-        <v>0.168279854614945</v>
+        <v>0.321582034841199</v>
       </c>
       <c r="C47">
-        <v>454.186159999013</v>
+        <v>50.0226708720351</v>
       </c>
       <c r="D47">
-        <v>417.541036183621</v>
+        <v>54.4925966516079</v>
       </c>
       <c r="E47">
-        <v>0.77188392639487</v>
-      </c>
-      <c r="F47">
-        <v>1</v>
+        <v>0.7529122425565569</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>PLCG2</t>
+          <t>MAF</t>
         </is>
       </c>
       <c r="B48">
-        <v>0.4776383080998</v>
+        <v>0.168279854614945</v>
       </c>
       <c r="C48">
-        <v>294.451133032978</v>
+        <v>454.186159999013</v>
       </c>
       <c r="D48">
-        <v>284.161441312083</v>
+        <v>417.541036183621</v>
       </c>
       <c r="E48">
-        <v>0.917035601118116</v>
-      </c>
-      <c r="F48">
-        <v>1</v>
+        <v>0.7494294275918612</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>WDR81</t>
+          <t>PLCG2</t>
         </is>
       </c>
       <c r="B49">
-        <v>0.265499155821289</v>
+        <v>0.4776383080998</v>
       </c>
       <c r="C49">
-        <v>33.091299067435</v>
+        <v>294.451133032978</v>
       </c>
       <c r="D49">
-        <v>34.7570200543969</v>
+        <v>284.161441312083</v>
       </c>
       <c r="E49">
-        <v>0.834344952739362</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
+        <v>0.7765096633414705</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>SCIMP</t>
+          <t>WDR81</t>
         </is>
       </c>
       <c r="B50">
-        <v>0.466994174145613</v>
+        <v>0.265499155821289</v>
       </c>
       <c r="C50">
-        <v>29.8110816310603</v>
+        <v>33.091299067435</v>
       </c>
       <c r="D50">
-        <v>30.4341023484971</v>
+        <v>34.7570200543969</v>
       </c>
       <c r="E50">
-        <v>0.912546554466398</v>
-      </c>
-      <c r="F50">
-        <v>1</v>
+        <v>0.7529122425565569</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>GRN</t>
+          <t>SCIMP</t>
         </is>
       </c>
       <c r="B51">
-        <v>0.0620970704808073</v>
+        <v>0.466994174145613</v>
       </c>
       <c r="C51">
-        <v>92.67480974273479</v>
+        <v>29.8110816310603</v>
       </c>
       <c r="D51">
-        <v>98.7267846015705</v>
+        <v>30.4341023484971</v>
       </c>
       <c r="E51">
-        <v>0.625199671065098</v>
-      </c>
-      <c r="F51">
-        <v>1</v>
+        <v>0.7765096633414705</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>ABI3</t>
+          <t>GRN</t>
         </is>
       </c>
       <c r="B52">
-        <v>0.186786400635221</v>
+        <v>0.0620970704808073</v>
       </c>
       <c r="C52">
-        <v>47.8717839627605</v>
+        <v>92.67480974273479</v>
       </c>
       <c r="D52">
-        <v>49.8034968836368</v>
+        <v>98.7267846015705</v>
       </c>
       <c r="E52">
-        <v>0.78735646252241</v>
-      </c>
-      <c r="F52">
-        <v>1</v>
+        <v>0.6963558963132086</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>TSPOAP1</t>
+          <t>ABI3</t>
         </is>
       </c>
       <c r="B53">
-        <v>0.548677517709573</v>
+        <v>0.186786400635221</v>
       </c>
       <c r="C53">
-        <v>26.4149914278373</v>
+        <v>47.8717839627605</v>
       </c>
       <c r="D53">
-        <v>28.9077647270305</v>
+        <v>49.8034968836368</v>
       </c>
       <c r="E53">
-        <v>0.935789102079309</v>
-      </c>
-      <c r="F53">
-        <v>1</v>
+        <v>0.7494294275918612</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ABCA7</t>
+          <t>TSPOAP1</t>
         </is>
       </c>
       <c r="B54">
-        <v>0.173220889338789</v>
+        <v>0.548677517709573</v>
       </c>
       <c r="C54">
-        <v>15.3067573542468</v>
+        <v>26.4149914278373</v>
       </c>
       <c r="D54">
-        <v>16.875518402004</v>
+        <v>28.9077647270305</v>
       </c>
       <c r="E54">
-        <v>0.777364940636564</v>
-      </c>
-      <c r="F54">
-        <v>1</v>
+        <v>0.8230162765643594</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>KLF16</t>
+          <t>ABCA7</t>
         </is>
       </c>
       <c r="B55">
-        <v>0.801433223600996</v>
+        <v>0.173220889338789</v>
       </c>
       <c r="C55">
-        <v>21.53256022097</v>
+        <v>15.3067573542468</v>
       </c>
       <c r="D55">
-        <v>22.0484566184267</v>
+        <v>16.875518402004</v>
       </c>
       <c r="E55">
-        <v>0.974845735941558</v>
-      </c>
-      <c r="F55">
-        <v>1</v>
+        <v>0.7494294275918612</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>SIGLEC11</t>
+          <t>KLF16</t>
         </is>
       </c>
       <c r="B56">
-        <v>0.761631431479593</v>
+        <v>0.801433223600996</v>
       </c>
       <c r="C56">
-        <v>25.6997992887589</v>
+        <v>21.53256022097</v>
       </c>
       <c r="D56">
-        <v>26.0625190461577</v>
+        <v>22.0484566184267</v>
       </c>
       <c r="E56">
-        <v>0.97005954789006</v>
-      </c>
-      <c r="F56">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>RBCK1</t>
+          <t>APOE</t>
         </is>
       </c>
       <c r="B57">
-        <v>0.891404907775894</v>
+        <v>0.0292861821589357</v>
       </c>
       <c r="C57">
-        <v>42.2493664469545</v>
+        <v>327.582149370953</v>
       </c>
       <c r="D57">
-        <v>41.7676885316144</v>
+        <v>365.931816251021</v>
       </c>
       <c r="E57">
-        <v>0.99063234765088</v>
-      </c>
-      <c r="F57">
-        <v>1</v>
+        <v>0.6963558963132086</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>CASS4</t>
+          <t>SIGLEC11</t>
         </is>
       </c>
       <c r="B58">
-        <v>0.856118755975664</v>
+        <v>0.761631431479593</v>
       </c>
       <c r="C58">
-        <v>56.5034249963918</v>
+        <v>25.6997992887589</v>
       </c>
       <c r="D58">
-        <v>56.2186134110797</v>
+        <v>26.0625190461577</v>
       </c>
       <c r="E58">
-        <v>0.985749275265047</v>
-      </c>
-      <c r="F58">
-        <v>1</v>
+        <v>0.9221430080440283</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
+          <t>RBCK1</t>
+        </is>
+      </c>
+      <c r="B59">
+        <v>0.891404907775894</v>
+      </c>
+      <c r="C59">
+        <v>42.2493664469545</v>
+      </c>
+      <c r="D59">
+        <v>41.7676885316144</v>
+      </c>
+      <c r="E59">
+        <v>0.9221430080440283</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>CASS4</t>
+        </is>
+      </c>
+      <c r="B60">
+        <v>0.856118755975664</v>
+      </c>
+      <c r="C60">
+        <v>56.5034249963918</v>
+      </c>
+      <c r="D60">
+        <v>56.2186134110797</v>
+      </c>
+      <c r="E60">
+        <v>0.9221430080440283</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
           <t>APP</t>
         </is>
       </c>
+      <c r="B61">
+        <v>0.285777318214529</v>
+      </c>
+      <c r="C61">
+        <v>217.788578337964</v>
+      </c>
+      <c r="D61">
+        <v>233.460874362011</v>
+      </c>
+      <c r="E61">
+        <v>0.7529122425565569</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>...1</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>logFC</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>logCPM</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>PValue</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>BHQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SORT1</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>0.0579064825831701</v>
+      </c>
+      <c r="C2">
+        <v>8.083803507936389</v>
+      </c>
+      <c r="D2">
+        <v>3.07891930832822</v>
+      </c>
+      <c r="E2">
+        <v>0.0800577229433265</v>
+      </c>
+      <c r="F2">
+        <v>0.6311258034231557</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ADAM17</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>0.0163716860044434</v>
+      </c>
+      <c r="C3">
+        <v>7.3395725903723</v>
+      </c>
+      <c r="D3">
+        <v>0.337005531889984</v>
+      </c>
+      <c r="E3">
+        <v>0.561880693935066</v>
+      </c>
+      <c r="F3">
+        <v>0.8639874600163739</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>PRKD3</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>-0.00275248050236068</v>
+      </c>
+      <c r="C4">
+        <v>7.69995301672174</v>
+      </c>
+      <c r="D4">
+        <v>0.00269425026370883</v>
+      </c>
+      <c r="E4">
+        <v>0.95862865660352</v>
+      </c>
+      <c r="F4">
+        <v>0.982533712568056</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>NCK2</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>-0.00637315674609176</v>
+      </c>
+      <c r="C5">
+        <v>9.30067150943057</v>
+      </c>
+      <c r="D5">
+        <v>0.009204636434787181</v>
+      </c>
+      <c r="E5">
+        <v>0.923614315876517</v>
+      </c>
+      <c r="F5">
+        <v>0.982533712568056</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BIN1</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>-0.134717934226917</v>
+      </c>
+      <c r="C6">
+        <v>8.392645940728791</v>
+      </c>
+      <c r="D6">
+        <v>4.07289605053545</v>
+      </c>
+      <c r="E6">
+        <v>0.0442251531597618</v>
+      </c>
+      <c r="F6">
+        <v>0.6311258034231557</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WDR12</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>-0.0336827302089642</v>
+      </c>
+      <c r="C7">
+        <v>5.50372169525649</v>
+      </c>
+      <c r="D7">
+        <v>0.46873492674499</v>
+      </c>
+      <c r="E7">
+        <v>0.493955308164289</v>
+      </c>
+      <c r="F7">
+        <v>0.7799294339436142</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>INPP5D</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>-0.0468935218772486</v>
+      </c>
+      <c r="C8">
+        <v>9.55921249918668</v>
+      </c>
+      <c r="D8">
+        <v>1.89696454295787</v>
+      </c>
+      <c r="E8">
+        <v>0.169167455093983</v>
+      </c>
+      <c r="F8">
+        <v>0.6521754331607886</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>IDUA</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>0.0364974273573777</v>
+      </c>
+      <c r="C9">
+        <v>4.31058146142589</v>
+      </c>
+      <c r="D9">
+        <v>0.3686374637973</v>
+      </c>
+      <c r="E9">
+        <v>0.697212689374119</v>
+      </c>
+      <c r="F9">
+        <v>0.9296169191654919</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>RHOH</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>-0.0550901831272309</v>
+      </c>
+      <c r="C10">
+        <v>5.95842265482306</v>
+      </c>
+      <c r="D10">
+        <v>0.845320690341711</v>
+      </c>
+      <c r="E10">
+        <v>0.35841830297375</v>
+      </c>
+      <c r="F10">
+        <v>0.6937128444653226</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ANKH</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>0.0450470264273717</v>
+      </c>
+      <c r="C11">
+        <v>7.26896994297913</v>
+      </c>
+      <c r="D11">
+        <v>1.48647175884213</v>
+      </c>
+      <c r="E11">
+        <v>0.223463365491905</v>
+      </c>
+      <c r="F11">
+        <v>0.6521754331607886</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>COX7C</t>
+        </is>
+      </c>
+      <c r="B12">
+        <v>-0.0412220633479878</v>
+      </c>
+      <c r="C12">
+        <v>7.29696851107268</v>
+      </c>
+      <c r="D12">
+        <v>0.57660185319047</v>
+      </c>
+      <c r="E12">
+        <v>0.448082305143308</v>
+      </c>
+      <c r="F12">
+        <v>0.7468038419055133</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TNIP1</t>
+        </is>
+      </c>
+      <c r="B13">
+        <v>0.0474892787373041</v>
+      </c>
+      <c r="C13">
+        <v>5.17538223690452</v>
+      </c>
+      <c r="D13">
+        <v>1.14354528833742</v>
+      </c>
+      <c r="E13">
+        <v>0.285531546666423</v>
+      </c>
+      <c r="F13">
+        <v>0.6937128444653226</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>RASGEF1C</t>
+        </is>
+      </c>
+      <c r="B14">
+        <v>-0.230118164330959</v>
+      </c>
+      <c r="C14">
+        <v>8.45180662580173</v>
+      </c>
+      <c r="D14">
+        <v>6.59059710459301</v>
+      </c>
+      <c r="E14">
+        <v>0.0106044670416894</v>
+      </c>
+      <c r="F14">
+        <v>0.318134011250682</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>HLA-DQA1</t>
+        </is>
+      </c>
+      <c r="B15">
+        <v>-0.0927523506696126</v>
+      </c>
+      <c r="C15">
+        <v>5.20623035296026</v>
+      </c>
+      <c r="D15">
+        <v>1.07106817464929</v>
+      </c>
+      <c r="E15">
+        <v>0.301312334567611</v>
+      </c>
+      <c r="F15">
+        <v>0.6937128444653226</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>TREM2</t>
+        </is>
+      </c>
+      <c r="B16">
+        <v>-0.00132040462997451</v>
+      </c>
+      <c r="C16">
+        <v>6.00156331544101</v>
+      </c>
+      <c r="D16">
+        <v>0.00047986449437469</v>
+      </c>
+      <c r="E16">
+        <v>0.982533712568056</v>
+      </c>
+      <c r="F16">
+        <v>0.982533712568056</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CD2AP</t>
+        </is>
+      </c>
+      <c r="B17">
+        <v>-0.0265918436355076</v>
+      </c>
+      <c r="C17">
+        <v>7.31245146105668</v>
+      </c>
+      <c r="D17">
+        <v>0.862772106289669</v>
+      </c>
+      <c r="E17">
+        <v>0.35350883549761</v>
+      </c>
+      <c r="F17">
+        <v>0.6937128444653226</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>UMAD1</t>
+        </is>
+      </c>
+      <c r="B18">
+        <v>-0.00198605609332365</v>
+      </c>
+      <c r="C18">
+        <v>7.94207562462902</v>
+      </c>
+      <c r="D18">
+        <v>0.00374131493168252</v>
+      </c>
+      <c r="E18">
+        <v>0.951256484348405</v>
+      </c>
+      <c r="F18">
+        <v>0.982533712568056</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ICA1</t>
+        </is>
+      </c>
+      <c r="B19">
+        <v>-0.0486812415557032</v>
+      </c>
+      <c r="C19">
+        <v>6.1718646474021</v>
+      </c>
+      <c r="D19">
+        <v>0.733069019562625</v>
+      </c>
+      <c r="E19">
+        <v>0.392388685024935</v>
+      </c>
+      <c r="F19">
+        <v>0.7301318362368636</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TMEM106B</t>
+        </is>
+      </c>
+      <c r="B20">
+        <v>-0.0123289573560747</v>
+      </c>
+      <c r="C20">
+        <v>5.99345188667036</v>
+      </c>
+      <c r="D20">
+        <v>0.094875118613161</v>
+      </c>
+      <c r="E20">
+        <v>0.758224508624087</v>
+      </c>
+      <c r="F20">
+        <v>0.9591744385420023</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>JAZF1</t>
+        </is>
+      </c>
+      <c r="B21">
+        <v>0.0892591010961554</v>
+      </c>
+      <c r="C21">
+        <v>9.9643944124604</v>
+      </c>
+      <c r="D21">
+        <v>2.88757046152163</v>
+      </c>
+      <c r="E21">
+        <v>0.09002149921740971</v>
+      </c>
+      <c r="F21">
+        <v>0.6311258034231557</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>EPDR1</t>
+        </is>
+      </c>
+      <c r="B22">
+        <v>0.00257010147283564</v>
+      </c>
+      <c r="C22">
+        <v>5.12806376266447</v>
+      </c>
+      <c r="D22">
+        <v>0.00144296774936892</v>
+      </c>
+      <c r="E22">
+        <v>0.969716941581239</v>
+      </c>
+      <c r="F22">
+        <v>0.982533712568056</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>SEC61G</t>
+        </is>
+      </c>
+      <c r="B23">
+        <v>-0.0318784495312308</v>
+      </c>
+      <c r="C23">
+        <v>5.08558526722334</v>
+      </c>
+      <c r="D23">
+        <v>0.265731648711253</v>
+      </c>
+      <c r="E23">
+        <v>0.606486429605371</v>
+      </c>
+      <c r="F23">
+        <v>0.8793112356123436</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>SPDYE3</t>
+        </is>
+      </c>
+      <c r="B24">
+        <v>-0.126210703455256</v>
+      </c>
+      <c r="C24">
+        <v>4.36751016246557</v>
+      </c>
+      <c r="D24">
+        <v>2.10831664263766</v>
+      </c>
+      <c r="E24">
+        <v>0.147262687465403</v>
+      </c>
+      <c r="F24">
+        <v>0.6311258034231557</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CTSB</t>
+        </is>
+      </c>
+      <c r="B25">
+        <v>-0.0196156582702717</v>
+      </c>
+      <c r="C25">
+        <v>9.043037002158719</v>
+      </c>
+      <c r="D25">
+        <v>0.212796368585749</v>
+      </c>
+      <c r="E25">
+        <v>0.644828239449052</v>
+      </c>
+      <c r="F25">
+        <v>0.8793112356123436</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>PTK2B</t>
+        </is>
+      </c>
+      <c r="B26">
+        <v>0.0167764607440006</v>
+      </c>
+      <c r="C26">
+        <v>7.56853751396274</v>
+      </c>
+      <c r="D26">
+        <v>0.2226968317339</v>
+      </c>
+      <c r="E26">
+        <v>0.637242934496584</v>
+      </c>
+      <c r="F26">
+        <v>0.8793112356123436</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CLU</t>
+        </is>
+      </c>
+      <c r="B27">
+        <v>0.0137711344391531</v>
+      </c>
+      <c r="C27">
+        <v>8.86489067334333</v>
+      </c>
+      <c r="D27">
+        <v>0.0559483799392089</v>
+      </c>
+      <c r="E27">
+        <v>0.813135991744621</v>
+      </c>
+      <c r="F27">
+        <v>0.9591744385420023</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>SHARPIN</t>
+        </is>
+      </c>
+      <c r="B28">
+        <v>-0.00773752206525446</v>
+      </c>
+      <c r="C28">
+        <v>4.80878140179818</v>
+      </c>
+      <c r="D28">
+        <v>0.0252269112392952</v>
+      </c>
+      <c r="E28">
+        <v>0.873880905526212</v>
+      </c>
+      <c r="F28">
+        <v>0.982533712568056</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ABCA1</t>
+        </is>
+      </c>
+      <c r="B29">
+        <v>0.0611877605284233</v>
+      </c>
+      <c r="C29">
+        <v>6.88541593268069</v>
+      </c>
+      <c r="D29">
+        <v>0.514830370717226</v>
+      </c>
+      <c r="E29">
+        <v>0.473462532890918</v>
+      </c>
+      <c r="F29">
+        <v>0.7677770803636509</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>USP6NL</t>
+        </is>
+      </c>
+      <c r="B30">
+        <v>0.0473384006502803</v>
+      </c>
+      <c r="C30">
+        <v>8.361449622919229</v>
+      </c>
+      <c r="D30">
+        <v>0.952061773166883</v>
+      </c>
+      <c r="E30">
+        <v>0.329768510598689</v>
+      </c>
+      <c r="F30">
+        <v>0.6937128444653226</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>ANK3</t>
+        </is>
+      </c>
+      <c r="B31">
+        <v>-0.0478174599882238</v>
+      </c>
+      <c r="C31">
+        <v>7.02926609187718</v>
+      </c>
+      <c r="D31">
+        <v>0.8895083020187891</v>
+      </c>
+      <c r="E31">
+        <v>0.346164186029556</v>
+      </c>
+      <c r="F31">
+        <v>0.6937128444653226</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>TSPAN14</t>
+        </is>
+      </c>
+      <c r="B32">
+        <v>0.0612326153897114</v>
+      </c>
+      <c r="C32">
+        <v>7.77065840316456</v>
+      </c>
+      <c r="D32">
+        <v>3.00298544176557</v>
+      </c>
+      <c r="E32">
+        <v>0.0838606970063078</v>
+      </c>
+      <c r="F32">
+        <v>0.6311258034231557</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>BLNK</t>
+        </is>
+      </c>
+      <c r="B33">
+        <v>-0.08889774263991471</v>
+      </c>
+      <c r="C33">
+        <v>8.769835916190379</v>
+      </c>
+      <c r="D33">
+        <v>2.31380515447961</v>
+      </c>
+      <c r="E33">
+        <v>0.128998106340457</v>
+      </c>
+      <c r="F33">
+        <v>0.6311258034231557</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>PLEKHA1</t>
+        </is>
+      </c>
+      <c r="B34">
+        <v>0.0487733830370746</v>
+      </c>
+      <c r="C34">
+        <v>6.6880252127416</v>
+      </c>
+      <c r="D34">
+        <v>1.77819550698002</v>
+      </c>
+      <c r="E34">
+        <v>0.183109016939943</v>
+      </c>
+      <c r="F34">
+        <v>0.6521754331607886</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>SPI1</t>
+        </is>
+      </c>
+      <c r="B35">
+        <v>-0.008822051981486719</v>
+      </c>
+      <c r="C35">
+        <v>6.48469935591825</v>
+      </c>
+      <c r="D35">
+        <v>0.0568147779978299</v>
+      </c>
+      <c r="E35">
+        <v>0.815298272760702</v>
+      </c>
+      <c r="F35">
+        <v>0.9591744385420023</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>MS4A4A</t>
+        </is>
+      </c>
+      <c r="B36">
+        <v>-0.0609921182900755</v>
+      </c>
+      <c r="C36">
+        <v>6.58070586055135</v>
+      </c>
+      <c r="D36">
+        <v>0.705071713043632</v>
+      </c>
+      <c r="E36">
+        <v>0.401572509930275</v>
+      </c>
+      <c r="F36">
+        <v>0.7301318362368636</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>EED</t>
+        </is>
+      </c>
+      <c r="B37">
+        <v>0.0412360566695458</v>
+      </c>
+      <c r="C37">
+        <v>6.32793602210925</v>
+      </c>
+      <c r="D37">
+        <v>0.994500695793869</v>
+      </c>
+      <c r="E37">
+        <v>0.319231118268529</v>
+      </c>
+      <c r="F37">
+        <v>0.6937128444653226</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>SORL1</t>
+        </is>
+      </c>
+      <c r="B38">
+        <v>-0.0368137090439273</v>
+      </c>
+      <c r="C38">
+        <v>10.4660717217936</v>
+      </c>
+      <c r="D38">
+        <v>0.620999680872322</v>
+      </c>
+      <c r="E38">
+        <v>0.431129918429551</v>
+      </c>
+      <c r="F38">
+        <v>0.7390798601649445</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>TPCN1</t>
+        </is>
+      </c>
+      <c r="B39">
+        <v>-0.0628572905009825</v>
+      </c>
+      <c r="C39">
+        <v>6.7369019991324</v>
+      </c>
+      <c r="D39">
+        <v>1.49000230018445</v>
+      </c>
+      <c r="E39">
+        <v>0.222915361164524</v>
+      </c>
+      <c r="F39">
+        <v>0.6521754331607886</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>FERMT2</t>
+        </is>
+      </c>
+      <c r="B40">
+        <v>0.106381225295906</v>
+      </c>
+      <c r="C40">
+        <v>4.60670148082872</v>
+      </c>
+      <c r="D40">
+        <v>2.26956931776916</v>
+      </c>
+      <c r="E40">
+        <v>0.132704106182422</v>
+      </c>
+      <c r="F40">
+        <v>0.6311258034231557</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>PSEN1</t>
+        </is>
+      </c>
+      <c r="B41">
+        <v>0.0275775161600033</v>
+      </c>
+      <c r="C41">
+        <v>7.02553030314467</v>
+      </c>
+      <c r="D41">
+        <v>0.907114752408315</v>
+      </c>
+      <c r="E41">
+        <v>0.341440431734869</v>
+      </c>
+      <c r="F41">
+        <v>0.6937128444653226</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>SPPL2A</t>
+        </is>
+      </c>
+      <c r="B42">
+        <v>0.0348744867443367</v>
+      </c>
+      <c r="C42">
+        <v>6.64371225097244</v>
+      </c>
+      <c r="D42">
+        <v>1.45599823953667</v>
+      </c>
+      <c r="E42">
+        <v>0.228261401606276</v>
+      </c>
+      <c r="F42">
+        <v>0.6521754331607886</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>MINDY2</t>
+        </is>
+      </c>
+      <c r="B43">
+        <v>0.0610347946824915</v>
+      </c>
+      <c r="C43">
+        <v>6.66797710213693</v>
+      </c>
+      <c r="D43">
+        <v>2.75702076056443</v>
+      </c>
+      <c r="E43">
+        <v>0.0975904445270136</v>
+      </c>
+      <c r="F43">
+        <v>0.6311258034231557</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>APH1B</t>
+        </is>
+      </c>
+      <c r="B44">
+        <v>0.0753924682890857</v>
+      </c>
+      <c r="C44">
+        <v>5.55846716141536</v>
+      </c>
+      <c r="D44">
+        <v>2.52466027273957</v>
+      </c>
+      <c r="E44">
+        <v>0.112847204257775</v>
+      </c>
+      <c r="F44">
+        <v>0.6311258034231557</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>SNX1</t>
+        </is>
+      </c>
+      <c r="B45">
+        <v>-0.00604940909460009</v>
+      </c>
+      <c r="C45">
+        <v>7.10928511887167</v>
+      </c>
+      <c r="D45">
+        <v>0.0560265214686719</v>
+      </c>
+      <c r="E45">
+        <v>0.813007966251608</v>
+      </c>
+      <c r="F45">
+        <v>0.9591744385420023</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CTSH</t>
+        </is>
+      </c>
+      <c r="B46">
+        <v>0.0105818675244234</v>
+      </c>
+      <c r="C46">
+        <v>6.46215589706811</v>
+      </c>
+      <c r="D46">
+        <v>0.0753714068294925</v>
+      </c>
+      <c r="E46">
+        <v>0.919676568697094</v>
+      </c>
+      <c r="F46">
+        <v>0.982533712568056</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>DOC2A</t>
+        </is>
+      </c>
+      <c r="B47">
+        <v>0.0600021814076994</v>
+      </c>
+      <c r="C47">
+        <v>5.81547393514325</v>
+      </c>
+      <c r="D47">
+        <v>0.9931126996822019</v>
+      </c>
+      <c r="E47">
+        <v>0.319568652130815</v>
+      </c>
+      <c r="F47">
+        <v>0.6937128444653226</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>MAF</t>
+        </is>
+      </c>
+      <c r="B48">
+        <v>-0.0909617167138095</v>
+      </c>
+      <c r="C48">
+        <v>8.73770435939211</v>
+      </c>
+      <c r="D48">
+        <v>2.7067550230724</v>
+      </c>
+      <c r="E48">
+        <v>0.100687956390456</v>
+      </c>
+      <c r="F48">
+        <v>0.6311258034231557</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>PLCG2</t>
+        </is>
+      </c>
+      <c r="B49">
+        <v>-0.0380334187218815</v>
+      </c>
+      <c r="C49">
+        <v>8.186915987039949</v>
+      </c>
+      <c r="D49">
+        <v>1.50104592309107</v>
+      </c>
+      <c r="E49">
+        <v>0.221211575593507</v>
+      </c>
+      <c r="F49">
+        <v>0.6521754331607886</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>WDR81</t>
+        </is>
+      </c>
+      <c r="B50">
+        <v>0.0393086071262568</v>
+      </c>
+      <c r="C50">
+        <v>5.22580381675462</v>
+      </c>
+      <c r="D50">
+        <v>0.663715080517275</v>
+      </c>
+      <c r="E50">
+        <v>0.418093940601755</v>
+      </c>
+      <c r="F50">
+        <v>0.7378128363560382</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>SCIMP</t>
+        </is>
+      </c>
+      <c r="B51">
+        <v>0.0304945505807605</v>
+      </c>
+      <c r="C51">
+        <v>5.0322368174412</v>
+      </c>
+      <c r="D51">
+        <v>0.223476587325047</v>
+      </c>
+      <c r="E51">
+        <v>0.636654333911237</v>
+      </c>
+      <c r="F51">
+        <v>0.8793112356123436</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>GRN</t>
+        </is>
+      </c>
+      <c r="B52">
+        <v>0.100930014163353</v>
+      </c>
+      <c r="C52">
+        <v>6.61435807866375</v>
+      </c>
+      <c r="D52">
+        <v>4.58365242870111</v>
+      </c>
+      <c r="E52">
+        <v>0.0328655358255854</v>
+      </c>
+      <c r="F52">
+        <v>0.6311258034231557</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>ABI3</t>
+        </is>
+      </c>
+      <c r="B53">
+        <v>0.0634374466081966</v>
+      </c>
+      <c r="C53">
+        <v>5.73565400391051</v>
+      </c>
+      <c r="D53">
+        <v>1.62880632670535</v>
+      </c>
+      <c r="E53">
+        <v>0.202588342222061</v>
+      </c>
+      <c r="F53">
+        <v>0.6521754331607886</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>TSPOAP1</t>
+        </is>
+      </c>
+      <c r="B54">
+        <v>0.0117570054927532</v>
+      </c>
+      <c r="C54">
+        <v>4.95709654157843</v>
+      </c>
+      <c r="D54">
+        <v>0.041144436335811</v>
+      </c>
+      <c r="E54">
+        <v>0.83935967176808</v>
+      </c>
+      <c r="F54">
+        <v>0.9684919289631692</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>ABCA7</t>
+        </is>
+      </c>
+      <c r="B55">
+        <v>0.107402011814522</v>
+      </c>
+      <c r="C55">
+        <v>4.3594951609163</v>
+      </c>
+      <c r="D55">
+        <v>2.1685212987717</v>
+      </c>
+      <c r="E55">
+        <v>0.141626345407227</v>
+      </c>
+      <c r="F55">
+        <v>0.6311258034231557</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>KLF16</t>
+        </is>
+      </c>
+      <c r="B56">
+        <v>0.0135515592076698</v>
+      </c>
+      <c r="C56">
+        <v>4.67843719794356</v>
+      </c>
+      <c r="D56">
+        <v>0.0609882150921785</v>
+      </c>
+      <c r="E56">
+        <v>0.805063994620593</v>
+      </c>
+      <c r="F56">
+        <v>0.9591744385420023</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>APOE</t>
+        </is>
+      </c>
+      <c r="B57">
+        <v>0.179133845374672</v>
+      </c>
+      <c r="C57">
+        <v>8.51991371625053</v>
+      </c>
+      <c r="D57">
+        <v>7.15411526023754</v>
+      </c>
+      <c r="E57">
+        <v>0.00777747402394618</v>
+      </c>
+      <c r="F57">
+        <v>0.318134011250682</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>SIGLEC11</t>
+        </is>
+      </c>
+      <c r="B58">
+        <v>0.0227109491061441</v>
+      </c>
+      <c r="C58">
+        <v>4.86411713208596</v>
+      </c>
+      <c r="D58">
+        <v>0.0735229388045872</v>
+      </c>
+      <c r="E58">
+        <v>0.7864108108028099</v>
+      </c>
+      <c r="F58">
+        <v>0.9591744385420023</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>RBCK1</t>
+        </is>
+      </c>
       <c r="B59">
-        <v>0.285777318214529</v>
+        <v>-0.00706027280497854</v>
       </c>
       <c r="C59">
-        <v>217.788578337964</v>
+        <v>5.50280440391886</v>
       </c>
       <c r="D59">
-        <v>233.460874362011</v>
+        <v>0.0350692457080711</v>
       </c>
       <c r="E59">
-        <v>0.8449618174724119</v>
+        <v>0.93303900785426</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>0.982533712568056</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>CASS4</t>
+        </is>
+      </c>
+      <c r="B60">
+        <v>-0.043634886049882</v>
+      </c>
+      <c r="C60">
+        <v>5.90171630270183</v>
+      </c>
+      <c r="D60">
+        <v>0.313259299355033</v>
+      </c>
+      <c r="E60">
+        <v>0.575991640010916</v>
+      </c>
+      <c r="F60">
+        <v>0.8639874600163739</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>APP</t>
+        </is>
+      </c>
+      <c r="B61">
+        <v>0.0382569918877195</v>
+      </c>
+      <c r="C61">
+        <v>7.82577878150947</v>
+      </c>
+      <c r="D61">
+        <v>0.935326697608322</v>
+      </c>
+      <c r="E61">
+        <v>0.33405086757999</v>
+      </c>
+      <c r="F61">
+        <v>0.6937128444653226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>